<commit_message>
Added fee comparison excel
</commit_message>
<xml_diff>
--- a/presentations/Comparativo de fees fijos y variables.xlsx
+++ b/presentations/Comparativo de fees fijos y variables.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andresp/Documents/R Projects/Trading bloque/presentations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2DB92D-DDFD-FA4D-B673-C951885210DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A207885-0BD7-B949-AE57-41AAA8662DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{FF18EC40-325D-4549-B661-1A48975C421C}"/>
   </bookViews>
   <sheets>
-    <sheet name="EQCHX" sheetId="2" r:id="rId1"/>
-    <sheet name="AQMIX" sheetId="1" r:id="rId2"/>
+    <sheet name="AQMIX (2)" sheetId="3" r:id="rId1"/>
+    <sheet name="EQCHX" sheetId="2" r:id="rId2"/>
+    <sheet name="AQMIX" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="new_sharpe" localSheetId="0">EQCHX!$C$14</definedName>
+    <definedName name="new_sharpe" localSheetId="0">'AQMIX (2)'!$C$14</definedName>
+    <definedName name="new_sharpe" localSheetId="1">EQCHX!$C$14</definedName>
     <definedName name="new_sharpe">AQMIX!$C$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="13">
   <si>
     <t>Retorno Neto</t>
   </si>
@@ -183,7 +185,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>EQCHX!$N$2</c:f>
+              <c:f>'AQMIX (2)'!$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -218,7 +220,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>EQCHX!$K$3:$K$12</c:f>
+              <c:f>'AQMIX (2)'!$K$3:$K$12</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
@@ -257,39 +259,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>EQCHX!$N$3:$N$12</c:f>
+              <c:f>'AQMIX (2)'!$N$3:$N$12</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>9.7999999999999962E-3</c:v>
+                  <c:v>4.7999999999999987E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.1750000000000017E-3</c:v>
+                  <c:v>2.8499999999999984E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.5500000000000003E-3</c:v>
+                  <c:v>8.9999999999999802E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.9249999999999988E-3</c:v>
+                  <c:v>-1.0500000000000093E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.2999999999999974E-3</c:v>
+                  <c:v>-3.0000000000000027E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6749999999999959E-3</c:v>
+                  <c:v>-4.9500000000000099E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.9999999999994493E-5</c:v>
+                  <c:v>-6.9000000000000034E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-1.5750000000000069E-3</c:v>
+                  <c:v>-8.8500000000000245E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-3.1999999999999945E-3</c:v>
+                  <c:v>-1.0799999999999976E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-4.8250000000000237E-3</c:v>
+                  <c:v>-1.2749999999999984E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -297,7 +299,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-222A-E942-AE5D-95DA7709A7C8}"/>
+              <c16:uniqueId val="{00000000-72F1-5942-88E8-5D092F31FDE2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -330,7 +332,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>EQCHX!$K$3:$K$12</c:f>
+              <c:f>'AQMIX (2)'!$K$3:$K$12</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
@@ -369,39 +371,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>EQCHX!$O$3:$O$12</c:f>
+              <c:f>'AQMIX (2)'!$O$3:$O$12</c:f>
               <c:numCache>
                 <c:formatCode>0.0000%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>-7.5999999999999991E-3</c:v>
+                  <c:v>-1.2599999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.14E-2</c:v>
+                  <c:v>-1.89E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.5199999999999998E-2</c:v>
+                  <c:v>-2.5199999999999993E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.8999999999999996E-2</c:v>
+                  <c:v>-3.1499999999999993E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-2.2800000000000001E-2</c:v>
+                  <c:v>-3.78E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-2.6599999999999999E-2</c:v>
+                  <c:v>-4.41E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3.0399999999999996E-2</c:v>
+                  <c:v>-5.0399999999999986E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-3.4199999999999994E-2</c:v>
+                  <c:v>-5.6699999999999987E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-3.7999999999999992E-2</c:v>
+                  <c:v>-6.2999999999999973E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-4.179999999999999E-2</c:v>
+                  <c:v>-6.9299999999999987E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -409,7 +411,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-222A-E942-AE5D-95DA7709A7C8}"/>
+              <c16:uniqueId val="{00000001-72F1-5942-88E8-5D092F31FDE2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -620,6 +622,1090 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>PIMCO Futures Fund: Sharpe 0.6x, Retorno anualizado 6.1%</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>vs.</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Fondo</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> con 0.5% de Management Fee, 13% de Performance</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+              <a:ea typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18132434494639219"/>
+          <c:y val="0.17560247133287446"/>
+          <c:w val="0.80768664406459678"/>
+          <c:h val="0.60632288501250764"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'AQMIX (2)'!$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sólo Management Fee</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="7030A0"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'AQMIX (2)'!$K$3:$K$12</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.5000000000000011E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.17499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.19999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.22499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.24999999999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.27499999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'AQMIX (2)'!$L$3:$L$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.5000000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.4999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.105</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.11999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.13499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.14999999999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.16499999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BBE8-F341-9108-F9E72403C926}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'AQMIX (2)'!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Performance Fee</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'AQMIX (2)'!$K$3:$K$12</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.5000000000000011E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.17499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.19999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.22499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.24999999999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.27499999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'AQMIX (2)'!$M$3:$M$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3.4799999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.7850000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0899999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3949999999999988E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.6999999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.10004999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.11309999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.12614999999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.13919999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.15225</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BBE8-F341-9108-F9E72403C926}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1848056064"/>
+        <c:axId val="1848070256"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1848056064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Volatilidad (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-AR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1848070256"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1848070256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Retorno Neto</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Anualizado (%)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-AR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1848056064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="5.000000000000001E-2"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-AR"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400">
+          <a:latin typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+          <a:ea typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-AR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>EQCHX!$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Manager 2 - Manager 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>EQCHX!$K$3:$K$12</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.5000000000000011E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.17499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.19999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.22499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.24999999999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.27499999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EQCHX!$N$3:$N$12</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9.7999999999999962E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.1750000000000017E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.5500000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.9249999999999988E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.2999999999999974E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6749999999999959E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.9999999999994493E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1.5750000000000069E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-3.1999999999999945E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-4.8250000000000237E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-222A-E942-AE5D-95DA7709A7C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>EQCHX!$K$3:$K$12</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.5000000000000011E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.17499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.19999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.22499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.24999999999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.27499999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EQCHX!$O$3:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-7.5999999999999991E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.14E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.5199999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.8999999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2.2800000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2.6599999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-3.0399999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-3.4199999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-3.7999999999999992E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-4.179999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-222A-E942-AE5D-95DA7709A7C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1167737232"/>
+        <c:axId val="1167717168"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1167737232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1167717168"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1167717168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1167737232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-AR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>Chesapeake Mutual Fund: Sharpe 0.5x, Retorno anualizado 7.3%</a:t>
             </a:r>
           </a:p>
@@ -1033,7 +2119,6 @@
         <c:axId val="1848070256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1145,7 +2230,7 @@
         <c:crossAx val="1848056064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="2.5000000000000005E-2"/>
+        <c:majorUnit val="3.7500000000000006E-2"/>
       </c:valAx>
       <c:dTable>
         <c:showHorzBorder val="1"/>
@@ -1242,7 +2327,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1669,7 +2754,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2480,6 +3565,83 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent5"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -4492,7 +5654,1164 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA102A61-5503-994E-8FD8-970DFCCED7DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E3A3B47-F266-EF4F-90B6-CE7D28C10E6F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Down Arrow 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88C3412B-0257-8641-B0B5-E658882AFA44}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7531100" y="3467100"/>
+          <a:ext cx="787400" cy="1092200"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="7030A0"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="vert270" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+              <a:ea typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Bookerly" panose="02020602040305020204" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>PIMCO</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4643,7 +6962,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5085,11 +7404,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9A36CB7-AE2F-424C-B896-E103D3F4D896}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E885FB2-F4F5-124C-BAE0-8F574778C02C}">
   <dimension ref="B1:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5162,14 +7481,14 @@
         <v>0.05</v>
       </c>
       <c r="C3" s="2">
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D3">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E3">
         <f>D3*B3</f>
-        <v>2.5000000000000001E-2</v>
+        <v>0.03</v>
       </c>
       <c r="F3" s="4">
         <f>E3+C3</f>
@@ -5195,7 +7514,7 @@
       </c>
       <c r="L3" s="7">
         <f>E3</f>
-        <v>2.5000000000000001E-2</v>
+        <v>0.03</v>
       </c>
       <c r="M3" s="7">
         <f>J3</f>
@@ -5203,11 +7522,11 @@
       </c>
       <c r="N3" s="1">
         <f>M3-L3</f>
-        <v>9.7999999999999962E-3</v>
+        <v>4.7999999999999987E-3</v>
       </c>
       <c r="O3" s="5">
         <f>Q3-L3</f>
-        <v>-7.5999999999999991E-3</v>
+        <v>-1.2599999999999997E-2</v>
       </c>
       <c r="P3">
         <f t="shared" ref="P3:P12" si="0">B3*new_sharpe</f>
@@ -5225,19 +7544,19 @@
       </c>
       <c r="C4" s="2">
         <f>C3</f>
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D4">
         <f>D3</f>
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E4">
         <f t="shared" ref="E4:E12" si="1">D4*B4</f>
-        <v>3.7500000000000006E-2</v>
+        <v>4.5000000000000005E-2</v>
       </c>
       <c r="F4" s="4">
         <f t="shared" ref="F4:F12" si="2">E4+C4</f>
-        <v>5.7500000000000009E-2</v>
+        <v>6.0000000000000005E-2</v>
       </c>
       <c r="G4" s="4">
         <f>G3</f>
@@ -5245,14 +7564,14 @@
       </c>
       <c r="H4" s="4">
         <f t="shared" ref="H4:H12" si="3">F4-G4</f>
-        <v>5.2500000000000012E-2</v>
+        <v>5.5000000000000007E-2</v>
       </c>
       <c r="I4" s="1">
         <v>0.13</v>
       </c>
       <c r="J4" s="5">
         <f t="shared" ref="J4:J12" si="4">H4*(1-I4)</f>
-        <v>4.5675000000000007E-2</v>
+        <v>4.7850000000000004E-2</v>
       </c>
       <c r="K4" s="1">
         <f t="shared" ref="K4:K12" si="5">B4</f>
@@ -5260,19 +7579,19 @@
       </c>
       <c r="L4" s="7">
         <f t="shared" ref="L4:L12" si="6">E4</f>
-        <v>3.7500000000000006E-2</v>
+        <v>4.5000000000000005E-2</v>
       </c>
       <c r="M4" s="7">
         <f t="shared" ref="M4:M12" si="7">J4</f>
-        <v>4.5675000000000007E-2</v>
+        <v>4.7850000000000004E-2</v>
       </c>
       <c r="N4" s="1">
         <f t="shared" ref="N4:N12" si="8">M4-L4</f>
-        <v>8.1750000000000017E-3</v>
+        <v>2.8499999999999984E-3</v>
       </c>
       <c r="O4" s="5">
         <f t="shared" ref="O4:O12" si="9">Q4-L4</f>
-        <v>-1.14E-2</v>
+        <v>-1.89E-2</v>
       </c>
       <c r="P4">
         <f t="shared" si="0"/>
@@ -5290,19 +7609,19 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ref="C5:D12" si="12">C4</f>
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D5">
         <f t="shared" si="12"/>
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="F5" s="4">
         <f t="shared" si="2"/>
-        <v>7.0000000000000007E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="G5" s="4">
         <f t="shared" ref="G5:G12" si="13">G4</f>
@@ -5310,14 +7629,14 @@
       </c>
       <c r="H5" s="4">
         <f t="shared" si="3"/>
-        <v>6.5000000000000002E-2</v>
+        <v>6.9999999999999993E-2</v>
       </c>
       <c r="I5" s="1">
         <v>0.13</v>
       </c>
       <c r="J5" s="5">
         <f t="shared" si="4"/>
-        <v>5.6550000000000003E-2</v>
+        <v>6.0899999999999996E-2</v>
       </c>
       <c r="K5" s="1">
         <f t="shared" si="5"/>
@@ -5325,19 +7644,19 @@
       </c>
       <c r="L5" s="7">
         <f t="shared" si="6"/>
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="M5" s="7">
         <f t="shared" si="7"/>
-        <v>5.6550000000000003E-2</v>
+        <v>6.0899999999999996E-2</v>
       </c>
       <c r="N5" s="1">
         <f t="shared" si="8"/>
-        <v>6.5500000000000003E-3</v>
+        <v>8.9999999999999802E-4</v>
       </c>
       <c r="O5" s="5">
         <f t="shared" si="9"/>
-        <v>-1.5199999999999998E-2</v>
+        <v>-2.5199999999999993E-2</v>
       </c>
       <c r="P5">
         <f t="shared" si="0"/>
@@ -5355,19 +7674,19 @@
       </c>
       <c r="C6" s="2">
         <f t="shared" si="12"/>
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D6">
         <f t="shared" si="12"/>
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="F6" s="4">
         <f t="shared" si="2"/>
-        <v>8.2500000000000004E-2</v>
+        <v>0.09</v>
       </c>
       <c r="G6" s="4">
         <f t="shared" si="13"/>
@@ -5375,14 +7694,14 @@
       </c>
       <c r="H6" s="4">
         <f t="shared" si="3"/>
-        <v>7.7499999999999999E-2</v>
+        <v>8.4999999999999992E-2</v>
       </c>
       <c r="I6" s="1">
         <v>0.13</v>
       </c>
       <c r="J6" s="5">
         <f t="shared" si="4"/>
-        <v>6.7424999999999999E-2</v>
+        <v>7.3949999999999988E-2</v>
       </c>
       <c r="K6" s="1">
         <f t="shared" si="5"/>
@@ -5390,19 +7709,19 @@
       </c>
       <c r="L6" s="7">
         <f t="shared" si="6"/>
-        <v>6.25E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="M6" s="7">
         <f t="shared" si="7"/>
-        <v>6.7424999999999999E-2</v>
+        <v>7.3949999999999988E-2</v>
       </c>
       <c r="N6" s="1">
         <f t="shared" si="8"/>
-        <v>4.9249999999999988E-3</v>
+        <v>-1.0500000000000093E-3</v>
       </c>
       <c r="O6" s="5">
         <f t="shared" si="9"/>
-        <v>-1.8999999999999996E-2</v>
+        <v>-3.1499999999999993E-2</v>
       </c>
       <c r="P6">
         <f t="shared" si="0"/>
@@ -5420,19 +7739,19 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" si="12"/>
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D7">
         <f t="shared" si="12"/>
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>7.4999999999999997E-2</v>
+        <v>0.09</v>
       </c>
       <c r="F7" s="4">
         <f t="shared" si="2"/>
-        <v>9.5000000000000001E-2</v>
+        <v>0.105</v>
       </c>
       <c r="G7" s="4">
         <f t="shared" si="13"/>
@@ -5440,14 +7759,14 @@
       </c>
       <c r="H7" s="4">
         <f t="shared" si="3"/>
-        <v>0.09</v>
+        <v>9.9999999999999992E-2</v>
       </c>
       <c r="I7" s="1">
         <v>0.13</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" si="4"/>
-        <v>7.8299999999999995E-2</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="K7" s="1">
         <f t="shared" si="5"/>
@@ -5455,19 +7774,19 @@
       </c>
       <c r="L7" s="7">
         <f t="shared" si="6"/>
-        <v>7.4999999999999997E-2</v>
+        <v>0.09</v>
       </c>
       <c r="M7" s="7">
         <f t="shared" si="7"/>
-        <v>7.8299999999999995E-2</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="N7" s="1">
         <f t="shared" si="8"/>
-        <v>3.2999999999999974E-3</v>
+        <v>-3.0000000000000027E-3</v>
       </c>
       <c r="O7" s="5">
         <f t="shared" si="9"/>
-        <v>-2.2800000000000001E-2</v>
+        <v>-3.78E-2</v>
       </c>
       <c r="P7">
         <f t="shared" si="0"/>
@@ -5485,19 +7804,19 @@
       </c>
       <c r="C8" s="2">
         <f t="shared" si="12"/>
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D8">
         <f t="shared" si="12"/>
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>8.7499999999999994E-2</v>
+        <v>0.105</v>
       </c>
       <c r="F8" s="4">
         <f t="shared" si="2"/>
-        <v>0.1075</v>
+        <v>0.12</v>
       </c>
       <c r="G8" s="4">
         <f t="shared" si="13"/>
@@ -5505,14 +7824,14 @@
       </c>
       <c r="H8" s="4">
         <f t="shared" si="3"/>
-        <v>0.10249999999999999</v>
+        <v>0.11499999999999999</v>
       </c>
       <c r="I8" s="1">
         <v>0.13</v>
       </c>
       <c r="J8" s="5">
         <f t="shared" si="4"/>
-        <v>8.917499999999999E-2</v>
+        <v>0.10004999999999999</v>
       </c>
       <c r="K8" s="1">
         <f t="shared" si="5"/>
@@ -5520,19 +7839,19 @@
       </c>
       <c r="L8" s="7">
         <f t="shared" si="6"/>
-        <v>8.7499999999999994E-2</v>
+        <v>0.105</v>
       </c>
       <c r="M8" s="7">
         <f t="shared" si="7"/>
-        <v>8.917499999999999E-2</v>
+        <v>0.10004999999999999</v>
       </c>
       <c r="N8" s="1">
         <f t="shared" si="8"/>
-        <v>1.6749999999999959E-3</v>
+        <v>-4.9500000000000099E-3</v>
       </c>
       <c r="O8" s="5">
         <f t="shared" si="9"/>
-        <v>-2.6599999999999999E-2</v>
+        <v>-4.41E-2</v>
       </c>
       <c r="P8">
         <f t="shared" si="0"/>
@@ -5550,19 +7869,19 @@
       </c>
       <c r="C9" s="2">
         <f t="shared" si="12"/>
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D9">
         <f t="shared" si="12"/>
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>9.9999999999999992E-2</v>
+        <v>0.11999999999999998</v>
       </c>
       <c r="F9" s="4">
         <f t="shared" si="2"/>
-        <v>0.12</v>
+        <v>0.13499999999999998</v>
       </c>
       <c r="G9" s="4">
         <f t="shared" si="13"/>
@@ -5570,14 +7889,14 @@
       </c>
       <c r="H9" s="4">
         <f t="shared" si="3"/>
-        <v>0.11499999999999999</v>
+        <v>0.12999999999999998</v>
       </c>
       <c r="I9" s="1">
         <v>0.13</v>
       </c>
       <c r="J9" s="5">
         <f t="shared" si="4"/>
-        <v>0.10004999999999999</v>
+        <v>0.11309999999999998</v>
       </c>
       <c r="K9" s="1">
         <f t="shared" si="5"/>
@@ -5585,19 +7904,19 @@
       </c>
       <c r="L9" s="7">
         <f t="shared" si="6"/>
-        <v>9.9999999999999992E-2</v>
+        <v>0.11999999999999998</v>
       </c>
       <c r="M9" s="7">
         <f t="shared" si="7"/>
-        <v>0.10004999999999999</v>
+        <v>0.11309999999999998</v>
       </c>
       <c r="N9" s="1">
         <f t="shared" si="8"/>
-        <v>4.9999999999994493E-5</v>
+        <v>-6.9000000000000034E-3</v>
       </c>
       <c r="O9" s="5">
         <f t="shared" si="9"/>
-        <v>-3.0399999999999996E-2</v>
+        <v>-5.0399999999999986E-2</v>
       </c>
       <c r="P9">
         <f t="shared" si="0"/>
@@ -5615,19 +7934,19 @@
       </c>
       <c r="C10" s="2">
         <f t="shared" si="12"/>
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D10">
         <f t="shared" si="12"/>
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>0.11249999999999999</v>
+        <v>0.13499999999999998</v>
       </c>
       <c r="F10" s="4">
         <f t="shared" si="2"/>
-        <v>0.13249999999999998</v>
+        <v>0.14999999999999997</v>
       </c>
       <c r="G10" s="4">
         <f t="shared" si="13"/>
@@ -5635,14 +7954,14 @@
       </c>
       <c r="H10" s="4">
         <f t="shared" si="3"/>
-        <v>0.12749999999999997</v>
+        <v>0.14499999999999996</v>
       </c>
       <c r="I10" s="1">
         <v>0.13</v>
       </c>
       <c r="J10" s="5">
         <f t="shared" si="4"/>
-        <v>0.11092499999999998</v>
+        <v>0.12614999999999996</v>
       </c>
       <c r="K10" s="1">
         <f t="shared" si="5"/>
@@ -5650,19 +7969,19 @@
       </c>
       <c r="L10" s="7">
         <f t="shared" si="6"/>
-        <v>0.11249999999999999</v>
+        <v>0.13499999999999998</v>
       </c>
       <c r="M10" s="7">
         <f t="shared" si="7"/>
-        <v>0.11092499999999998</v>
+        <v>0.12614999999999996</v>
       </c>
       <c r="N10" s="1">
         <f t="shared" si="8"/>
-        <v>-1.5750000000000069E-3</v>
+        <v>-8.8500000000000245E-3</v>
       </c>
       <c r="O10" s="5">
         <f t="shared" si="9"/>
-        <v>-3.4199999999999994E-2</v>
+        <v>-5.6699999999999987E-2</v>
       </c>
       <c r="P10">
         <f t="shared" si="0"/>
@@ -5680,19 +7999,19 @@
       </c>
       <c r="C11" s="2">
         <f t="shared" si="12"/>
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D11">
         <f t="shared" si="12"/>
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>0.12499999999999999</v>
+        <v>0.14999999999999997</v>
       </c>
       <c r="F11" s="4">
         <f t="shared" si="2"/>
-        <v>0.14499999999999999</v>
+        <v>0.16499999999999998</v>
       </c>
       <c r="G11" s="4">
         <f t="shared" si="13"/>
@@ -5700,14 +8019,14 @@
       </c>
       <c r="H11" s="4">
         <f t="shared" si="3"/>
-        <v>0.13999999999999999</v>
+        <v>0.15999999999999998</v>
       </c>
       <c r="I11" s="1">
         <v>0.13</v>
       </c>
       <c r="J11" s="5">
         <f t="shared" si="4"/>
-        <v>0.12179999999999999</v>
+        <v>0.13919999999999999</v>
       </c>
       <c r="K11" s="1">
         <f t="shared" si="5"/>
@@ -5715,19 +8034,19 @@
       </c>
       <c r="L11" s="7">
         <f t="shared" si="6"/>
-        <v>0.12499999999999999</v>
+        <v>0.14999999999999997</v>
       </c>
       <c r="M11" s="7">
         <f t="shared" si="7"/>
-        <v>0.12179999999999999</v>
+        <v>0.13919999999999999</v>
       </c>
       <c r="N11" s="1">
         <f t="shared" si="8"/>
-        <v>-3.1999999999999945E-3</v>
+        <v>-1.0799999999999976E-2</v>
       </c>
       <c r="O11" s="5">
         <f t="shared" si="9"/>
-        <v>-3.7999999999999992E-2</v>
+        <v>-6.2999999999999973E-2</v>
       </c>
       <c r="P11">
         <f t="shared" si="0"/>
@@ -5745,19 +8064,19 @@
       </c>
       <c r="C12" s="2">
         <f t="shared" si="12"/>
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D12">
         <f t="shared" si="12"/>
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>0.13749999999999998</v>
+        <v>0.16499999999999998</v>
       </c>
       <c r="F12" s="4">
         <f t="shared" si="2"/>
-        <v>0.15749999999999997</v>
+        <v>0.18</v>
       </c>
       <c r="G12" s="4">
         <f t="shared" si="13"/>
@@ -5765,14 +8084,14 @@
       </c>
       <c r="H12" s="4">
         <f t="shared" si="3"/>
-        <v>0.15249999999999997</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="I12" s="1">
         <v>0.13</v>
       </c>
       <c r="J12" s="5">
         <f t="shared" si="4"/>
-        <v>0.13267499999999996</v>
+        <v>0.15225</v>
       </c>
       <c r="K12" s="1">
         <f t="shared" si="5"/>
@@ -5780,19 +8099,19 @@
       </c>
       <c r="L12" s="7">
         <f t="shared" si="6"/>
-        <v>0.13749999999999998</v>
+        <v>0.16499999999999998</v>
       </c>
       <c r="M12" s="7">
         <f t="shared" si="7"/>
-        <v>0.13267499999999996</v>
+        <v>0.15225</v>
       </c>
       <c r="N12" s="1">
         <f t="shared" si="8"/>
-        <v>-4.8250000000000237E-3</v>
+        <v>-1.2749999999999984E-2</v>
       </c>
       <c r="O12" s="5">
         <f t="shared" si="9"/>
-        <v>-4.179999999999999E-2</v>
+        <v>-6.9299999999999987E-2</v>
       </c>
       <c r="P12">
         <f t="shared" si="0"/>
@@ -5815,11 +8134,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4835053-7857-D046-93FA-3694651831AC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9A36CB7-AE2F-424C-B896-E103D3F4D896}">
   <dimension ref="B1:Q14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5892,6 +8211,736 @@
         <v>0.05</v>
       </c>
       <c r="C3" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="D3">
+        <v>0.5</v>
+      </c>
+      <c r="E3">
+        <f>D3*B3</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F3" s="4">
+        <f>E3+C3</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="G3" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H3" s="4">
+        <f>F3-G3</f>
+        <v>0.04</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="J3" s="5">
+        <f>H3*(1-I3)</f>
+        <v>3.4799999999999998E-2</v>
+      </c>
+      <c r="K3" s="1">
+        <f>B3</f>
+        <v>0.05</v>
+      </c>
+      <c r="L3" s="7">
+        <f>E3</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M3" s="7">
+        <f>J3</f>
+        <v>3.4799999999999998E-2</v>
+      </c>
+      <c r="N3" s="1">
+        <f>M3-L3</f>
+        <v>9.7999999999999962E-3</v>
+      </c>
+      <c r="O3" s="5">
+        <f>Q3-L3</f>
+        <v>-7.5999999999999991E-3</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P12" si="0">B3*new_sharpe</f>
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="Q3" s="5">
+        <f>P3*(1-I3)</f>
+        <v>1.7400000000000002E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B4" s="3">
+        <f>B3+2.5%</f>
+        <v>7.5000000000000011E-2</v>
+      </c>
+      <c r="C4" s="2">
+        <f>C3</f>
+        <v>0.02</v>
+      </c>
+      <c r="D4">
+        <f>D3</f>
+        <v>0.5</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E12" si="1">D4*B4</f>
+        <v>3.7500000000000006E-2</v>
+      </c>
+      <c r="F4" s="4">
+        <f t="shared" ref="F4:F12" si="2">E4+C4</f>
+        <v>5.7500000000000009E-2</v>
+      </c>
+      <c r="G4" s="4">
+        <f>G3</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H4" s="4">
+        <f t="shared" ref="H4:H12" si="3">F4-G4</f>
+        <v>5.2500000000000012E-2</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="J4" s="5">
+        <f t="shared" ref="J4:J12" si="4">H4*(1-I4)</f>
+        <v>4.5675000000000007E-2</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" ref="K4:K12" si="5">B4</f>
+        <v>7.5000000000000011E-2</v>
+      </c>
+      <c r="L4" s="7">
+        <f t="shared" ref="L4:L12" si="6">E4</f>
+        <v>3.7500000000000006E-2</v>
+      </c>
+      <c r="M4" s="7">
+        <f t="shared" ref="M4:M12" si="7">J4</f>
+        <v>4.5675000000000007E-2</v>
+      </c>
+      <c r="N4" s="1">
+        <f t="shared" ref="N4:N12" si="8">M4-L4</f>
+        <v>8.1750000000000017E-3</v>
+      </c>
+      <c r="O4" s="5">
+        <f t="shared" ref="O4:O12" si="9">Q4-L4</f>
+        <v>-1.14E-2</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="Q4" s="5">
+        <f t="shared" ref="Q4:Q12" si="10">P4*(1-I4)</f>
+        <v>2.6100000000000005E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B5" s="3">
+        <f t="shared" ref="B5:B11" si="11">B4+2.5%</f>
+        <v>0.1</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" ref="C5:D12" si="12">C4</f>
+        <v>0.02</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="F5" s="4">
+        <f t="shared" si="2"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" ref="G5:G12" si="13">G4</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H5" s="4">
+        <f t="shared" si="3"/>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="J5" s="5">
+        <f t="shared" si="4"/>
+        <v>5.6550000000000003E-2</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="5"/>
+        <v>0.1</v>
+      </c>
+      <c r="L5" s="7">
+        <f t="shared" si="6"/>
+        <v>0.05</v>
+      </c>
+      <c r="M5" s="7">
+        <f t="shared" si="7"/>
+        <v>5.6550000000000003E-2</v>
+      </c>
+      <c r="N5" s="1">
+        <f t="shared" si="8"/>
+        <v>6.5500000000000003E-3</v>
+      </c>
+      <c r="O5" s="5">
+        <f t="shared" si="9"/>
+        <v>-1.5199999999999998E-2</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="Q5" s="5">
+        <f t="shared" si="10"/>
+        <v>3.4800000000000005E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B6" s="3">
+        <f t="shared" si="11"/>
+        <v>0.125</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" si="12"/>
+        <v>0.02</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F6" s="4">
+        <f t="shared" si="2"/>
+        <v>8.2500000000000004E-2</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="13"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H6" s="4">
+        <f t="shared" si="3"/>
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="J6" s="5">
+        <f t="shared" si="4"/>
+        <v>6.7424999999999999E-2</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" si="5"/>
+        <v>0.125</v>
+      </c>
+      <c r="L6" s="7">
+        <f t="shared" si="6"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="M6" s="7">
+        <f t="shared" si="7"/>
+        <v>6.7424999999999999E-2</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" si="8"/>
+        <v>4.9249999999999988E-3</v>
+      </c>
+      <c r="O6" s="5">
+        <f t="shared" si="9"/>
+        <v>-1.8999999999999996E-2</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
+      <c r="Q6" s="5">
+        <f t="shared" si="10"/>
+        <v>4.3500000000000004E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B7" s="3">
+        <f t="shared" si="11"/>
+        <v>0.15</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" si="12"/>
+        <v>0.02</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F7" s="4">
+        <f t="shared" si="2"/>
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="13"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H7" s="4">
+        <f t="shared" si="3"/>
+        <v>0.09</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="J7" s="5">
+        <f t="shared" si="4"/>
+        <v>7.8299999999999995E-2</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="5"/>
+        <v>0.15</v>
+      </c>
+      <c r="L7" s="7">
+        <f t="shared" si="6"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="M7" s="7">
+        <f t="shared" si="7"/>
+        <v>7.8299999999999995E-2</v>
+      </c>
+      <c r="N7" s="1">
+        <f t="shared" si="8"/>
+        <v>3.2999999999999974E-3</v>
+      </c>
+      <c r="O7" s="5">
+        <f t="shared" si="9"/>
+        <v>-2.2800000000000001E-2</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>0.06</v>
+      </c>
+      <c r="Q7" s="5">
+        <f t="shared" si="10"/>
+        <v>5.2199999999999996E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B8" s="3">
+        <f t="shared" si="11"/>
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" si="12"/>
+        <v>0.02</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="F8" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1075</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="13"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H8" s="4">
+        <f t="shared" si="3"/>
+        <v>0.10249999999999999</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" si="4"/>
+        <v>8.917499999999999E-2</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="5"/>
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="L8" s="7">
+        <f t="shared" si="6"/>
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="M8" s="7">
+        <f t="shared" si="7"/>
+        <v>8.917499999999999E-2</v>
+      </c>
+      <c r="N8" s="1">
+        <f t="shared" si="8"/>
+        <v>1.6749999999999959E-3</v>
+      </c>
+      <c r="O8" s="5">
+        <f t="shared" si="9"/>
+        <v>-2.6599999999999999E-2</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>6.9999999999999993E-2</v>
+      </c>
+      <c r="Q8" s="5">
+        <f t="shared" si="10"/>
+        <v>6.0899999999999996E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B9" s="3">
+        <f t="shared" si="11"/>
+        <v>0.19999999999999998</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" si="12"/>
+        <v>0.02</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="F9" s="4">
+        <f t="shared" si="2"/>
+        <v>0.12</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="13"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H9" s="4">
+        <f t="shared" si="3"/>
+        <v>0.11499999999999999</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="J9" s="5">
+        <f t="shared" si="4"/>
+        <v>0.10004999999999999</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" si="5"/>
+        <v>0.19999999999999998</v>
+      </c>
+      <c r="L9" s="7">
+        <f t="shared" si="6"/>
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="M9" s="7">
+        <f t="shared" si="7"/>
+        <v>0.10004999999999999</v>
+      </c>
+      <c r="N9" s="1">
+        <f t="shared" si="8"/>
+        <v>4.9999999999994493E-5</v>
+      </c>
+      <c r="O9" s="5">
+        <f t="shared" si="9"/>
+        <v>-3.0399999999999996E-2</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>0.08</v>
+      </c>
+      <c r="Q9" s="5">
+        <f t="shared" si="10"/>
+        <v>6.9599999999999995E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B10" s="3">
+        <f t="shared" si="11"/>
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" si="12"/>
+        <v>0.02</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>0.11249999999999999</v>
+      </c>
+      <c r="F10" s="4">
+        <f t="shared" si="2"/>
+        <v>0.13249999999999998</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="13"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H10" s="4">
+        <f t="shared" si="3"/>
+        <v>0.12749999999999997</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="J10" s="5">
+        <f t="shared" si="4"/>
+        <v>0.11092499999999998</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" si="5"/>
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="L10" s="7">
+        <f t="shared" si="6"/>
+        <v>0.11249999999999999</v>
+      </c>
+      <c r="M10" s="7">
+        <f t="shared" si="7"/>
+        <v>0.11092499999999998</v>
+      </c>
+      <c r="N10" s="1">
+        <f t="shared" si="8"/>
+        <v>-1.5750000000000069E-3</v>
+      </c>
+      <c r="O10" s="5">
+        <f t="shared" si="9"/>
+        <v>-3.4199999999999994E-2</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>0.09</v>
+      </c>
+      <c r="Q10" s="5">
+        <f t="shared" si="10"/>
+        <v>7.8299999999999995E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B11" s="3">
+        <f t="shared" si="11"/>
+        <v>0.24999999999999997</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" si="12"/>
+        <v>0.02</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>0.12499999999999999</v>
+      </c>
+      <c r="F11" s="4">
+        <f t="shared" si="2"/>
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="13"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H11" s="4">
+        <f t="shared" si="3"/>
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="J11" s="5">
+        <f t="shared" si="4"/>
+        <v>0.12179999999999999</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" si="5"/>
+        <v>0.24999999999999997</v>
+      </c>
+      <c r="L11" s="7">
+        <f t="shared" si="6"/>
+        <v>0.12499999999999999</v>
+      </c>
+      <c r="M11" s="7">
+        <f t="shared" si="7"/>
+        <v>0.12179999999999999</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="8"/>
+        <v>-3.1999999999999945E-3</v>
+      </c>
+      <c r="O11" s="5">
+        <f t="shared" si="9"/>
+        <v>-3.7999999999999992E-2</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="Q11" s="5">
+        <f t="shared" si="10"/>
+        <v>8.6999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B12" s="3">
+        <f>B11+2.5%</f>
+        <v>0.27499999999999997</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="12"/>
+        <v>0.02</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>0.13749999999999998</v>
+      </c>
+      <c r="F12" s="4">
+        <f t="shared" si="2"/>
+        <v>0.15749999999999997</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="13"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H12" s="4">
+        <f t="shared" si="3"/>
+        <v>0.15249999999999997</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="J12" s="5">
+        <f t="shared" si="4"/>
+        <v>0.13267499999999996</v>
+      </c>
+      <c r="K12" s="1">
+        <f t="shared" si="5"/>
+        <v>0.27499999999999997</v>
+      </c>
+      <c r="L12" s="7">
+        <f t="shared" si="6"/>
+        <v>0.13749999999999998</v>
+      </c>
+      <c r="M12" s="7">
+        <f t="shared" si="7"/>
+        <v>0.13267499999999996</v>
+      </c>
+      <c r="N12" s="1">
+        <f t="shared" si="8"/>
+        <v>-4.8250000000000237E-3</v>
+      </c>
+      <c r="O12" s="5">
+        <f t="shared" si="9"/>
+        <v>-4.179999999999999E-2</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>0.10999999999999999</v>
+      </c>
+      <c r="Q12" s="5">
+        <f t="shared" si="10"/>
+        <v>9.5699999999999993E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C14" s="6">
+        <v>0.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4835053-7857-D046-93FA-3694651831AC}">
+  <dimension ref="B1:Q14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="str">
+        <f>C2</f>
+        <v>Management Fee</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" t="str">
+        <f>" @ Sharpe de "&amp;new_sharpe&amp;" y Performance de "&amp;+TEXT(I3,"##%")</f>
+        <v xml:space="preserve"> @ Sharpe de 0.4 y Performance de 13%</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B3" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C3" s="2">
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="D3">

</xml_diff>